<commit_message>
functions to improve the code
</commit_message>
<xml_diff>
--- a/respuestas/registro/registro.xlsx
+++ b/respuestas/registro/registro.xlsx
@@ -459,7 +459,7 @@
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col width="21.140625" customWidth="1" min="4" max="4"/>
     <col width="19.5703125" customWidth="1" min="5" max="5"/>
@@ -1028,25 +1028,275 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>sdas</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Soltero</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>sdas</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Soltero</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>sdas</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Soltero</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Casado</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>asdasdasd</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2022-02-10</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Casado</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Add button for second exam
</commit_message>
<xml_diff>
--- a/respuestas/registro/registro.xlsx
+++ b/respuestas/registro/registro.xlsx
@@ -1303,6 +1303,56 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>asdas</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>dasda</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>sdasdasd</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2022-02-09</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Casado</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>asdasd</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">

</xml_diff>